<commit_message>
Borrar contenido doc Criterios de aceptacion
</commit_message>
<xml_diff>
--- a/Archivos_imp/test.xlsx
+++ b/Archivos_imp/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HISTORIA DE USUARIO" sheetId="1" state="visible" r:id="rId1"/>
@@ -1290,14 +1290,14 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2034,7 +2034,7 @@
   <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -2178,209 +2178,206 @@
       </c>
       <c r="B7" s="152" t="inlineStr">
         <is>
-          <t>Visualizar los correos internos agrupados  por TAGS</t>
+          <t>Registrar Correo interno</t>
         </is>
       </c>
       <c r="C7" s="152" t="inlineStr">
         <is>
-          <t>Dado que el usuario con el perfil “Cliente” se encuentra en el Controlador principal del cliente &gt; Envíos físicos &gt;   “Correo Interno”,</t>
+          <t>Dado que el usuario se encuentra en la pantalla principal del sistema, cuando hace clic en la Opción para crear un “Correo Interno” (Ver Pantalla principal),</t>
         </is>
       </c>
       <c r="D7" s="152" t="inlineStr">
         <is>
-          <t>Entonces el sistema:
-Mostrará un listado de “Correos internos”  agrupados en un TAG según su estado actual.
-Se mostrarán sólo los TAGs que contengan al menos un registro.
-El usuario podrá hacer clic en cualquier TAG y el sistema mostrará el listado de envíos que correspondan con el TAG seleccionado. Los tags se definen en la Tabla Estados y Tags Correo Interno - Cliente
-El usuario con perfil “Cliente” no podrá visualizar los envíos en estado “Anulado”.
-Se mostrará el conteo de envíos para cada estado, a excepción de la opción “Todos”
-En la Ruta de “Miga de pan” se mostrará el “TAG” donde se encuentra ubicado el usuario.
-En la tabla que despliega los envíos, diferenciar los estados por color.</t>
+          <t>1. El sistema deberá mostrar una nueva pantalla “Nuevo envío de correo interno” donde se podrá visualizar los campos requeridos para registrar un correo interno  (Correo Interno).
+2. Si el rol del usuario es “Back Office”, en la pantalla de “Nuevo envío de correo interno” se mostrará el campo adicional “Recogido”, el cual es un campo de selección para que el operador pueda marcar si el envío ya se encuentra en Cartería, lo que significa que NO hay que recogerlo.
+3.  Si el rol del usuario es “Cliente”,  en la pantalla de  “Nuevo envío de correo interno” No se mostrará el campo adicional “Recogido”.
+4. El “tipo de envío” para un Envío de correo interno siempre es “Correo interno”.
+5. Al documento físico el operador le puede  asignar un “Código QR” físicamente, el código QR se captura al hacer el registro del correo interno.</t>
         </is>
       </c>
       <c r="E7" s="152" t="inlineStr">
         <is>
-          <t>Estados/TAGs que visualizarán los usuarios (Registrador CI /Remitente/Destinatario) en la interfaz  del “cliente destinatario”:
-Todos
-Pte. Recoger
-En tránsito
-En custodia
-En distribución
-Entregado
-Incidencia
-Los TAGs se definen según el estado del envío así:
-Columnas a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO: Muestra el “Identificador del envío”.
-Información secundaria: 
-Código QR del envío.
-Tipo de envío:  Muestra el “Tipo de envío”.
-Información secundaria:
-“Creado”: Fecha-hora de creación del envío.
-Remitente: 
-Si el remitente es un “usuario” se muestra  el nombre + apellidos del usuario 
-Información secundaria:
-Se muestra el departamento asociado al usuario al momento de crear el envío.
-Si el remitente es un “departamento” se muestra directamente el nombre del departamento. 
-Información secundaria:
-No se muestra información secundaria.
-Formato de Recogida: Muestra el formato de recogida del envío.
-Ubicación Recogida:  Muestra la información de la ubicación del punto de entrega del remitente para la recogida. se deben mostrar los siguientes datos:
+          <t>Campos para el registro del envío:
+Datos de recogida
+Remitente
+Departamento (solo consulta)
+Formato de recogida 
+Ubicación: (solo consulta)
+Mostrar datos del punto de entrega del remitente para la recogida):
 PTOENTREGA.NOMBRE
-Información secundaria:
+PTOENTREGA.CODIGO
+EDIFICIO.NOMBRE
+PTOENTREGA.PLANTA
+PTOENTREGA.UBICACIÓN
+EDIFICIO.POBLACIÓN
+Ejemplo remitente tipo Usuario:
+Remitente: Sergi González [Dpto]
+Formato Recogida: En Bandeja
+Ubicación: [Datos del punto de entrega del Remitente] 
+Datos del destinatario
+Destinatario 
+Departamento (solo consulta)
+Formato de entrega  (solo consulta)
+Ubicación: (solo consulta)
+Mostrar datos del punto de entrega del destinatario:
+PTOENTREGA.NOMBRE
 PTOENTREGA.CODIGO
 EDIFICIO.NOMBRE
 PTOENTREGA.PLANTA
 PTOENTREGA.UBICACION
 EDIFICIO.POBLACION
-2024-07-16 se adiciona condiciones para la ubicación del remitente
-Para el punto de entrega (ubicación recogida) del remitente se debe tener en cuenta el estado actual del envío:
-Si el estado actual del envío se encuentra configurado dentro de los estados de envío que requieren que se guarde el punto de entrega del "Remitente" en las recogidas (correo interno, salidas) al momento de la asignación del estado  [Recepcionado] se debe mostrar el “punto de entrega” que se almacenó en la “Trazabilidad de estados”  que corresponda a dicho estado.  
-Si el estado actual del envío NO se encuentra configurado dentro de los estados que requieren que se guarde el punto de entrega del "Remitente" se debe mostrar el “punto de entrega” actual del Remitente.
-Nota: estos estados de envío que se configuren como que requieren almacenar el "punto de entrega" deben ser dinámicos, es decir que en cualquier momento deben poder adicionarse/quitarse estados que requieran almacenar este dato.
-Destinatario:  
-Si el destinatario es un “usuario” se muestra  el nombre + apellidos del usuario.
-Información secundaria:
-Se muestra el departamento asociado al usuario al momento de crear el envío.
-Si el destinatario es un “departamento” se muestra directamente el nombre del departamento. 
-Información secundaria:
-No se muestra información secundaria.
-Formato de Entrega: Muestra el formato de entrega del envío.
-Ubicación Entrega:  Muestra la información de la ubicación del punto de entrega del destinatario para la entrega. se deben mostrar los siguientes datos:
+Ejemplo Destinatario tipo Usuario:
+Destinatario: Tomas Borras [Dpto]
+Formato Entrega: En Bandeja
+Ubicación: [Datos del punto de entrega del Destinatario]
+Otros campos
+Código QR
+Recogido (Checkbox). Aplica para el Back Office
+Observaciones
+Botones:
+Cancelar 
+Crear envío</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="14.4" customHeight="1" s="212">
+      <c r="A8" s="147" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+      <c r="B8" s="152" t="inlineStr">
+        <is>
+          <t>Guardar envío &gt; Asignación de estado inicial del envío según check de “Recogido”</t>
+        </is>
+      </c>
+      <c r="C8" s="152" t="inlineStr">
+        <is>
+          <t>Dado que el usuario se encuentra en la interfaz de registro de “Correo Interno”,  cuando el diligencie los campos y presione el botón “Crear envío” o  "Crear y Agregar Otro",</t>
+        </is>
+      </c>
+      <c r="D8" s="152" t="inlineStr">
+        <is>
+          <t>1. Si el campo “Recogido” NO está marcado,  significa  que el envío debe recogerse por cartería (“En mano” o “En punto de entrega”) o que el remitente lo debe depositar en cartería (“En cartería”), en este caso se asigna el estado del envío a “Pte. de recoger”  (Ver Flujo Estados Correo Interno).
+2. En caso contrario, si el campo “Recogido” está marcado,  significa  que el envío ya se encuentra en cartería. Entonces, el sistema almacena el estado inicial del envío correspondiente a “Recepcionado”, y automáticamente se continúa el flujo dependiendo de la “Regla de envío” configurada para el tipo de ítem y el destinatario del envío (departamento / departamento del usuario)</t>
+        </is>
+      </c>
+      <c r="E8" s="152" t="inlineStr">
+        <is>
+          <t>Botón Crear envío</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="14.4" customHeight="1" s="212">
+      <c r="A9" s="147" t="inlineStr">
+        <is>
+          <t>03</t>
+        </is>
+      </c>
+      <c r="B9" s="152" t="inlineStr">
+        <is>
+          <t>Guardar envío &gt; Se define el “Estado del envío” dependiendo del destinatario (departamento/departamento del usuario)  y el Tipo de envío.</t>
+        </is>
+      </c>
+      <c r="C9" s="152" t="inlineStr">
+        <is>
+          <t>Dado que el usuario se encuentra en la interfaz de registro de “Correo Interno”,  cuando el diligencie los campos y presione el botón “Crear envío” o  "Crear y Agregar Otro",</t>
+        </is>
+      </c>
+      <c r="D9" s="152" t="inlineStr">
+        <is>
+          <t>Si el campo “Recogido” NO está marcado (el envío no debe recogerse por cartería) y dependiendo del Tipo de envío y el destinatario (departamento / departamento del usuario) elegidos al crear el correo interno, el sistema obtendrá la “Regla del Envío” correspondiente a correo interno (HU-080 Configuración de Reglas de ítem)  donde el sistema automáticamente valida:
+Si  el destinatario es de otro operativo (edificio de otra cartería ), entonces: 
+El envío pasa a estado de “Pte. Reexpedir" y sigue el flujo de correo interno (Ver Flujo Estados Correo Interno)
+Si el destinatario no es de otro operativo, entonces:
+Se definirá el flujo a llevar a cabo para la entrega del envío, de acuerdo al flujo que aplique se asignará el nuevo estado del envío  (Ver Flujo Estados Correo Interno).
+Si el destinatario es un “Usuario” se tiene en cuenta el “punto de entrega” definido por el propio usuario.
+Si el destinatario es un “Departamento” será el “punto de entrega” definido para ese departamento.</t>
+        </is>
+      </c>
+      <c r="E9" s="152" t="inlineStr">
+        <is>
+          <t>Botón Crear envío</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="14.4" customHeight="1" s="212">
+      <c r="A10" s="147" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+      <c r="B10" s="152" t="inlineStr">
+        <is>
+          <t>Guardar envío &gt; 
+Aceptar proceso de crear correo interno</t>
+        </is>
+      </c>
+      <c r="C10" s="152" t="inlineStr">
+        <is>
+          <t>Dado que el usuario se encuentra en la interfaz de registro de “Correo Interno”,  cuando el diligencie los campos y presione el botón “Crear envío” o  "Crear y Agregar Otro",</t>
+        </is>
+      </c>
+      <c r="D10" s="152" t="inlineStr">
+        <is>
+          <t>El sistema debe asegurar que:
+Se cumpla con todas las validaciones de la tabla “Detalle de Campos”.
+No se viola la integridad de la información.
+En caso que:
+Se cumpla con todas las validaciones, el sistema debe permitir guardar la información en la Base de Datos.
+A. El sistema debe guardar los siguientes campos de forma automática:
+Identificador GIO: Este campo debe ser único, autoincremental  y no se debe repetir para otro registro dentro del mismo Partner.
+Fecha y hora de creación: fecha y hora de creación del envío. Se debe almacenar/mostrar la correspondiente a la población del operativo que tiene asignado el envío cuando se realiza la acción concreta. Se debe tener en cuenta que en varios países se cambia la hora según sea horario de verano o invierno.
+Método de generación: Medio por el cuál se registra el envío (Manual)
+Estado del envío: Se guarda automáticamente dependiendo del flujo del diagrama de correo interno (Ver Flujo Estados Correo Interno).
+Id del Perfil del usuario: Id del Perfil del usuario que registra el envío.
+Id del Nombre de Usuario (username): Id del Nombre de usuario que registra el envío. Se guardará el ID interno del usuario, no el username ya que este puede variar.
+Punto de entrega: Punto de entrega del destinatario, al momento del registro del  envío. se deben guardar los siguientes datos:
 PTOENTREGA.NOMBRE
-Información secundaria:
 PTOENTREGA.CODIGO
 EDIFICIO.NOMBRE
 PTOENTREGA.PLANTA
-PTOENTREGA.UBICACION
+PTOENTREGA.UBICACIÓN
 EDIFICIO.POBLACION
-2024-07-16 se adiciona condiciones para la ubicación del destinatario
-Para el punto de entrega (ubicación entrega) del destinatario se debe tener en cuenta el estado actual del envío:
-Si el estado actual del envío se encuentra configurado dentro de los estados de envío que requieren que se guarde el punto de entrega del "Destinatario" en las entregas (entrada, correo interno) al momento de la asignación del estado  [Extraviado, Entregado, Anulado, Archivo Definitivo, Devolución] se debe mostrar el “punto de entrega” que se almacenó en la “Trazabilidad de estados”  que corresponda a dicho estado.  
-Si el estado actual del envío NO se encuentra configurado dentro de los estados que requieren que se guarde el punto de entrega del "Destinatario" se debe mostrar el “punto de entrega” actual del destinatario.
+Nota: El punto de entrega para la recogida será el que tenga el usuario en el momento en que se realice la Ronda de recogida(no impacta la presente HU).
+Formato de entrega: Se debe guardar el formato de entrega, ya que la regla del envío puede cambiar o eliminarse.
+Formato de recogida:Se debe guardar el formato de recogida, ya que la regla del envío puede cambiar o eliminarse.
+Id del departamento: 
+Id del departamento del remitente.
+ Id del departamento del destinatario.
+Id del Operativo: 
+Si es un envío registrado por el BackOffice: operativo al que pertenece el Back Office, hace referencia al Operativo desde el que se ha realizado la acción. Esto implica que un Back Office que tenga más de un operativo asignado deberá elegir en qué operativo va a operar al momento de iniciar sesión en el sistema.
+Si es un envío registrado por el Cliente:  Operativo que gestiona el edificio al que corresponde el punto de entrega del usuario remitente del correo interno.
+Id de la regla del envío (antes llamada regla de ítem) debe guardar toda la información de la regla de envío seleccionada, estos campos se almacenan en caso tal que la regla de envío cambie o se elimine.
+Acción según el botón seleccionado:
+Si el usuario oprime el botón "Crear Envio", el sistema informa al usuario que el "Envío se ha registrado correctamente con el ID XXXXXXXX" y dirige al usuario a la Pantalla principal del cliente o backoffice dependiendo del perfil del usuario logueado.
+Si el usuario oprime el botón "Crear y Agregar Otro", el sistema informa al usuario que el "Envío se ha registrado correctamente con el ID XXXXXXXX" y se "limpia" el formulario para permitirle al usuario registrar un nuevo Envío de correo interno, esto con el fin de que se puedan registrar varios Envíos de forma consecutiva.
+B. Trazabilidad
+El sistema automáticamente almacena la trazabilidad de los estados asignados al envío, se guarda información como:
+Fecha y hora (de la asignación del estado del envío). Se debe almacenar y mostrar la fecha/hora correspondiente a la población del operativo que tiene asignado el envío cuando se ha realizado la acción concreta. También hay que tener en cuenta que por ejemplo en muchos países se cambia la hora según sea horario de verano o invierno.
+    Nota: Lo anterior aplica a todos los eventos realizados con los envíos que supongan un cambio de estado, iniciar una ronda, etc.
+Nombre del estado asignado al envío.
+Usuario que realiza la acción que ocasiona la asignación del estado.
+Id del Perfil del usuario: Id del Perfil del usuario que registra el envío.
+Operativo:
+Si es un envío registrado por el BackOffice: operativo al que pertenece el Back Office, hace referencia al Operativo desde el que se ha realizado la acción. Esto implica que un Back Office que tenga más de un operativo asignado deberá elegir en qué operativo va a operar al momento de iniciar sesión en el sistema.
+Si es un envío registrado por el Cliente:  Operativo que gestiona el edificio al que corresponde el punto de entrega del usuario remitente del correo interno.
+2024-07-16
+2. Verificar si la trazabilidad  del estado requiere almacenar Punto de entrega
+Verificar si al almacenar la trazabilidad del estado se requiere almacenar el "Punto de entrega" teniendo en cuenta lo siguiente:
+ESTADOS_TRAZABILIDAD_PUNTO_ENTREGA_ENTREGAS: Estados de envío que requieren que se guarde el punto de entrega del "Destinatario" en las entregas (entrada, correo interno) al momento de la asignación del estado al envío.
+[Extraviado, Entregado, Anulado, Archivo Definitivo, Devolución]
+ESTADOS_TRAZABILIDAD_PUNTO_ENTREGA_RECOGIDAS: Estados que requieren que se guarde el "Punto de entrega" del "Remitente" en las recogidas (correo interno, salidas) al momento de la asignación del estado.
+[Recepcionado]
 Nota: estos estados de envío que se configuren como que requieren almacenar el "punto de entrega" deben ser dinámicos, es decir que en cualquier momento deben poder adicionarse/quitarse estados que requieran almacenar este dato.
-Estado:   Muestra el “Estado” actual del envío.
-Información secundaria:
-Fecha y hora en la que se asignó el estado del envío.
-Acciones individuales específicas: Muestra las acciones individuales específicas que podrá realizar el usuario para un envío dependiendo de su estado actual (estas acciones se especifican para cada estado en los siguientes criterios de aceptación).</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="14.4" customHeight="1" s="212">
-      <c r="A8" s="147" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="B8" s="152" t="inlineStr">
-        <is>
-          <t>Configurar columnas dinamicas</t>
-        </is>
-      </c>
-      <c r="C8" s="152" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” de cualquier estado y desea personalizar las columnas del listado,</t>
-        </is>
-      </c>
-      <c r="D8" s="152" t="inlineStr">
-        <is>
-          <t>Los campos (columnas) que se muestran en el listado serán dinámicos, es decir, el usuario podrá configurar las columnas que desea ver o ocultar en el listado. Se activa HU-204 Configurar Columnas Dinámicas en Listados.</t>
-        </is>
-      </c>
-      <c r="E8" s="152" t="inlineStr">
-        <is>
-          <t>Botón:
-Columnas</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="14.4" customHeight="1" s="212">
-      <c r="A9" s="147" t="inlineStr">
-        <is>
-          <t>03</t>
-        </is>
-      </c>
-      <c r="B9" s="152" t="inlineStr">
-        <is>
-          <t>Visualizar “Todos” los registros de Correo interno</t>
-        </is>
-      </c>
-      <c r="C9" s="152" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” del estado &gt; Todos,</t>
-        </is>
-      </c>
-      <c r="D9" s="152" t="inlineStr">
-        <is>
-          <t>El sistema mostrará un listado que incluirá todos los correos internos.
-En esta opción no se contempla el conteo de envíos. 
-Los envíos en estado “Entregado” que han cumplido el tiempo configurado para archivo  se verán en “Todos”, según lo definido en la HU-049 Configuración de preferencias de Archivo  (Cliente).
-En la tabla que despliega los envíos, diferenciar los estados por color.
-Los envíos en estado “Anulado” podrán ser vistos solo por el “BackOffice”, estos no se verán por el “Cliente".
-Los envíos en estado “Reexpedido” cuando son entregados en el destino, funcionan con la regla de archivo de los entregados para ir a “Todos”, según lo definido en la HU-049 Configuración de preferencias de Archivo  (Cliente)
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado actual del envío.
-Los envíos en estado “Extraviado” podrán ser vistos por el “Cliente” en la sección “Todos”, estos no se verán en un estado aparte en el listado.
-Los envíos en estado “Devolución” podrán ser vistos por el “Cliente” en la sección “Todos”, estos no se verán en un estado aparte en el listado.</t>
-        </is>
-      </c>
-      <c r="E9" s="152" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Todos los estados a excepción del estado “Anulado” )
-Acciones individuales específicas: Muestra el listado de acciones que podrá realizar el usuario dependiendo del estado del envío, por ejemplo:
-Mensaje a cartería
-Crear Incidencia (aplica para el estado diferente a incidencia) (estas acciones se especifican para cada estado en los siguientes criterios de aceptación).</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="14.4" customHeight="1" s="212">
-      <c r="A10" s="147" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
-      </c>
-      <c r="B10" s="152" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos que se encuentran en estado “Pte. Recoger”</t>
-        </is>
-      </c>
-      <c r="C10" s="152" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Pte. Recoger,</t>
-        </is>
-      </c>
-      <c r="D10" s="152" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos que están en estado “Pte. Recoger” por parte de Cartería.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Pte. Recoger” las etiquetas o tag que verá el usuario son:
-Registrador CI: Pte. de recoger
-Remitente: Pte. de recoger
-Destinatario: Pte. de recoger</t>
+3. La trazabilidad de los estados del envío se muestra en la sección de trazabilidad del envío (HU-024 Ver Trazabilidad del Correo Interno)
+No se cumpla con al menos una validación, el sistema no debe permitir guardar la información en la Base de Datos.
+Nota: En la tabla (Estados /TAG Correo Interno) se explican los “Tags” o “Estados” de cómo se visualizará el envío en los listados tanto para los usuarios (Back Office y Cliente) origen y destino.</t>
         </is>
       </c>
       <c r="E10" s="152" t="inlineStr">
         <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Pte. Recoger)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
+          <t>Botón “Crear envío”</t>
         </is>
       </c>
     </row>
@@ -2392,39 +2389,22 @@
       </c>
       <c r="B11" s="152" t="inlineStr">
         <is>
-          <t>Visualizar los correos internos en estado “Recepcionado”</t>
+          <t>Cancelar el proceso de registrar un correo interno</t>
         </is>
       </c>
       <c r="C11" s="152" t="inlineStr">
         <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Recepcionado,</t>
+          <t>Dado que el usuario está creando un “Correo interno” (Correo Interno) y el usuario desea cerrar el modal, cuando le da clic en el botón “Cancelar”,</t>
         </is>
       </c>
       <c r="D11" s="152" t="inlineStr">
         <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos en estado “Recepcionado” con sus respectivos detalles. 
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Recepcionado” las etiquetas o tag que verá el usuario son:
-Registrador CI: En tránsito
-Remitente: En tránsito
-Destinatario: En tránsito</t>
+          <t>Al salir de un formulario en creación con cambios pendientes el sistema debe preguntar al usuario si desea salir sin guardar o permanecer en la página “¿Desea salir sin guardar los cambios?” [Aceptar] Salir sin guardar [Cancelar] Permanecer en el formulario.</t>
         </is>
       </c>
       <c r="E11" s="152" t="inlineStr">
         <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Recepcionado)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
+          <t>Botón: Cancelar.</t>
         </is>
       </c>
     </row>
@@ -2436,41 +2416,20 @@
       </c>
       <c r="B12" s="152" t="inlineStr">
         <is>
-          <t>Visualizar los correos internos en estado “En custodia”</t>
+          <t>Cliente de cartería inmobiliaria</t>
         </is>
       </c>
       <c r="C12" s="152" t="inlineStr">
         <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno”&gt; para los envíos en estado En custodia,</t>
+          <t>Dado que el “Usuario” está asociado a una cuenta cliente de tipo “Cartería inmobiliaria”,</t>
         </is>
       </c>
       <c r="D12" s="152" t="inlineStr">
         <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos en estado  “En custodia” con sus respectivos detalles.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “En custodia” las etiquetas o tag que verá el usuario son:
-Registrador CI: En custodia
-Remitente: En custodia
-Destinatario: En custodia</t>
-        </is>
-      </c>
-      <c r="E12" s="152" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (En Custodia)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
-        </is>
-      </c>
+          <t>En el sistema la funcionalidad de “Registrar correo interno” no debe estar  disponible para “Usuarios” que pertenecen a cuentas de tipo “Cartería inmobiliaria”.</t>
+        </is>
+      </c>
+      <c r="E12" s="152" t="n"/>
     </row>
     <row r="13" ht="14.4" customHeight="1" s="212">
       <c r="A13" s="147" t="inlineStr">
@@ -2478,43 +2437,10 @@
           <t>07</t>
         </is>
       </c>
-      <c r="B13" s="148" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “Pte. Distribución”</t>
-        </is>
-      </c>
-      <c r="C13" s="148" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Pte. Distribución,</t>
-        </is>
-      </c>
-      <c r="D13" s="150" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos en estado  “Pte. Distribución” con sus respectivos detalles.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Pte. Distribución” las etiquetas o tag que verá el usuario son:
-Registrador CI: En tránsito
-Remitente: En tránsito
-Destinatario: En tránsito</t>
-        </is>
-      </c>
-      <c r="E13" s="150" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Pte. de distribución)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
-        </is>
-      </c>
+      <c r="B13" s="148" t="n"/>
+      <c r="C13" s="148" t="n"/>
+      <c r="D13" s="150" t="n"/>
+      <c r="E13" s="150" t="n"/>
     </row>
     <row r="14" ht="14.4" customHeight="1" s="212">
       <c r="A14" s="147" t="inlineStr">
@@ -2522,43 +2448,10 @@
           <t>08</t>
         </is>
       </c>
-      <c r="B14" s="148" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “En distribución”</t>
-        </is>
-      </c>
-      <c r="C14" s="149" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno”&gt; para los envíos en estado  En distribución,</t>
-        </is>
-      </c>
-      <c r="D14" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos en estado  “En distribución” con sus respectivos detalles.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “En  Distribución” las etiquetas o tag que verá el usuario son:
-Registrador CI: En distribución
-Remitente: En distribución
-Destinatario: En distribución</t>
-        </is>
-      </c>
-      <c r="E14" s="32" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (En Distribución)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
-        </is>
-      </c>
+      <c r="B14" s="148" t="n"/>
+      <c r="C14" s="149" t="n"/>
+      <c r="D14" s="32" t="n"/>
+      <c r="E14" s="32" t="n"/>
     </row>
     <row r="15" ht="14.4" customHeight="1" s="212">
       <c r="A15" s="147" t="inlineStr">
@@ -2566,45 +2459,10 @@
           <t>09</t>
         </is>
       </c>
-      <c r="B15" s="126" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “Entregado”</t>
-        </is>
-      </c>
-      <c r="C15" s="149" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Entregado,</t>
-        </is>
-      </c>
-      <c r="D15" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado que mostrará los correos internos en estado “Entregado” con sus respectivos detalles. 
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Entregado” las etiquetas o tag que verá el usuario son:
-Registrador CI: Entregado
-Remitente: Entregado
-Destinatario: Entregado
-En esta sección el sistema debe mostrar los correos internos en estado entregado que aún no han sido archivadas, de acuerdo con la configuración de Archivo establecida en la HU-049 Configuración de preferencias de Archivo  (Cliente).
-Los envíos en estado “Reexpedido” cuando son entregados en el destino, funcionan con la regla de archivo de los entregados para ir a “Todos”, según lo definido en la HU-049 Configuración de preferencias de Archivo  (Cliente).</t>
-        </is>
-      </c>
-      <c r="E15" s="32" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Entregado)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
-        </is>
-      </c>
+      <c r="B15" s="126" t="n"/>
+      <c r="C15" s="149" t="n"/>
+      <c r="D15" s="32" t="n"/>
+      <c r="E15" s="32" t="n"/>
     </row>
     <row r="16" ht="14.4" customHeight="1" s="212">
       <c r="A16" s="147" t="inlineStr">
@@ -2612,43 +2470,10 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B16" s="148" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “Pte. Reexpedir”</t>
-        </is>
-      </c>
-      <c r="C16" s="149" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Pte. Reexpedir,</t>
-        </is>
-      </c>
-      <c r="D16" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos que están en estado “Pte. Reexpedir”.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Pte. Reexpedir” las etiquetas o tag que verá el usuario son:
-Registrador CI: En tránsito
-Remitente: En tránsito
-Destinatario: En tránsito</t>
-        </is>
-      </c>
-      <c r="E16" s="32" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Pte. Reexpedir)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear Incidencia</t>
-        </is>
-      </c>
+      <c r="B16" s="148" t="n"/>
+      <c r="C16" s="149" t="n"/>
+      <c r="D16" s="32" t="n"/>
+      <c r="E16" s="32" t="n"/>
     </row>
     <row r="17" ht="14.4" customHeight="1" s="212">
       <c r="A17" s="147" t="inlineStr">
@@ -2656,43 +2481,10 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B17" s="148" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “Reexpedido”</t>
-        </is>
-      </c>
-      <c r="C17" s="149" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno”&gt; para los envíos en estado  Reexpedido,</t>
-        </is>
-      </c>
-      <c r="D17" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos que están en estado “Reexpedido”.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Reexpedido” las etiquetas o tag que verá el usuario son:
-Registrador CI: En tránsito
-Remitente: En tránsito
-Destinatario: En tránsito</t>
-        </is>
-      </c>
-      <c r="E17" s="32" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Reexpedido)
-Acciones individuales específicas:
-Mensaje a cartería
-Crear incidencia</t>
-        </is>
-      </c>
+      <c r="B17" s="148" t="n"/>
+      <c r="C17" s="149" t="n"/>
+      <c r="D17" s="32" t="n"/>
+      <c r="E17" s="32" t="n"/>
     </row>
     <row r="18" ht="14.4" customHeight="1" s="212">
       <c r="A18" s="147" t="inlineStr">
@@ -2700,43 +2492,10 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B18" s="126" t="inlineStr">
-        <is>
-          <t>Visualizar los correos internos en estado “Incidencia”</t>
-        </is>
-      </c>
-      <c r="C18" s="149" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra visualizando el listado de envíos de “Correo Interno” &gt; para los envíos en estado Incidencia,</t>
-        </is>
-      </c>
-      <c r="D18" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá desplegar un listado donde mostrará los correos internos están en estado “Incidencia”.
-En la “zona activa” donde se muestran los envíos en la columna “Estado” se mostrará el estado real del envío.
-Dado que el estado del envío está en “Incidencia” las etiquetas o tag que verá el usuario son:
-Registrador CI: Incidencia
-Remitente: Incidencia
-Destinatario: Incidencia
-Para los envíos en estado “Incidencia” no se habilita la acción “Crear incidencia”.</t>
-        </is>
-      </c>
-      <c r="E18" s="32" t="inlineStr">
-        <is>
-          <t>Campos a mostrar por defecto (si el usuario no ha personalizado los campos a mostrar):
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado (Estado actual de la última incidencia del envío)
-Acciones individuales específicas:
-Mensaje a cartería</t>
-        </is>
-      </c>
+      <c r="B18" s="126" t="n"/>
+      <c r="C18" s="149" t="n"/>
+      <c r="D18" s="32" t="n"/>
+      <c r="E18" s="32" t="n"/>
     </row>
     <row r="19" ht="14.4" customHeight="1" s="212">
       <c r="A19" s="147" t="inlineStr">
@@ -2744,21 +2503,9 @@
           <t>13</t>
         </is>
       </c>
-      <c r="B19" s="148" t="inlineStr">
-        <is>
-          <t>Correos Internos que se encuentran en estado “Anulado”</t>
-        </is>
-      </c>
-      <c r="C19" s="148" t="inlineStr">
-        <is>
-          <t>Dado que el usuario "Cliente" se encuentra en la Pantalla  “Correo Interno” &gt; para los envíos en estado  Anulado,</t>
-        </is>
-      </c>
-      <c r="D19" s="32" t="inlineStr">
-        <is>
-          <t>Los correos internos con estado "Anulado" no se visualizarán en la interfaz del “Cliente”, estos envíos podrán ser vistos SOLO por el “Back Office” de cartería en el TAG “Todos”.</t>
-        </is>
-      </c>
+      <c r="B19" s="148" t="n"/>
+      <c r="C19" s="148" t="n"/>
+      <c r="D19" s="32" t="n"/>
       <c r="E19" s="32" t="n"/>
     </row>
     <row r="20">
@@ -2767,24 +2514,9 @@
           <t>14</t>
         </is>
       </c>
-      <c r="B20" s="148" t="inlineStr">
-        <is>
-          <t>Correos Internos que se encuentran en estado “Extraviado”</t>
-        </is>
-      </c>
-      <c r="C20" s="148" t="inlineStr">
-        <is>
-          <t>Dado que el usuario "Cliente" se encuentra en la Pantalla  “Correo Interno” y desea ver los envíos con estado  “Extraviado”,</t>
-        </is>
-      </c>
-      <c r="D20" s="32" t="inlineStr">
-        <is>
-          <t>Los correos internos con estado "Extraviado" podrán ser vistos en la interfaz de “Cliente” de cartería en el TAG “Todos”, así:
-Registrador CI: Todos
-Remitente: Todos
-Destinatario: Todos</t>
-        </is>
-      </c>
+      <c r="B20" s="148" t="n"/>
+      <c r="C20" s="148" t="n"/>
+      <c r="D20" s="32" t="n"/>
       <c r="E20" s="32" t="n"/>
     </row>
     <row r="21">
@@ -2793,24 +2525,9 @@
           <t>15</t>
         </is>
       </c>
-      <c r="B21" s="148" t="inlineStr">
-        <is>
-          <t>Correos Internos que se encuentran en estado “Devolución”</t>
-        </is>
-      </c>
-      <c r="C21" s="148" t="inlineStr">
-        <is>
-          <t>Dado que el usuario "Cliente" se encuentra en la Pantalla  “Correo Interno” y desea ver los envíos con estado “Devolución”,</t>
-        </is>
-      </c>
-      <c r="D21" s="32" t="inlineStr">
-        <is>
-          <t>Los correos internos con estado "Devolución" podrán ser vistos en la interfaz de “Cliente” de cartería en el TAG “Todos”, así:
-Registrador CI: Todos
-Remitente: Todos
-Destinatario: Todos</t>
-        </is>
-      </c>
+      <c r="B21" s="148" t="n"/>
+      <c r="C21" s="148" t="n"/>
+      <c r="D21" s="32" t="n"/>
       <c r="E21" s="32" t="n"/>
     </row>
     <row r="22">
@@ -2819,21 +2536,9 @@
           <t>16</t>
         </is>
       </c>
-      <c r="B22" s="148" t="inlineStr">
-        <is>
-          <t>Ver detalle del envío</t>
-        </is>
-      </c>
-      <c r="C22" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno”, visualizando el listado de envíos de cualquier estado, cuando haga clic en un envío en específico,</t>
-        </is>
-      </c>
-      <c r="D22" s="32" t="inlineStr">
-        <is>
-          <t>El sistema mostrará información con el detalle del envío seleccionado. Se Activa la HU-023 Ver Detalle del Correo Interno Seleccionado</t>
-        </is>
-      </c>
+      <c r="B22" s="148" t="n"/>
+      <c r="C22" s="32" t="n"/>
+      <c r="D22" s="32" t="n"/>
       <c r="E22" s="32" t="n"/>
     </row>
     <row r="23">
@@ -2842,27 +2547,10 @@
           <t>17</t>
         </is>
       </c>
-      <c r="B23" s="148" t="inlineStr">
-        <is>
-          <t>Acción “Mensaje a Cartería”</t>
-        </is>
-      </c>
-      <c r="C23" s="126" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno”, visualizando el listado de envíos de cualquier tag/estado, cuando haga clic en la acción “Mensaje a cartería” de un registro,</t>
-        </is>
-      </c>
-      <c r="D23" s="32" t="inlineStr">
-        <is>
-          <t>Se Activa la HU-009 Enviar Mensaje a Cartería (Acción)</t>
-        </is>
-      </c>
-      <c r="E23" s="32" t="inlineStr">
-        <is>
-          <t>Acción
-Mensaje a cartería</t>
-        </is>
-      </c>
+      <c r="B23" s="148" t="n"/>
+      <c r="C23" s="126" t="n"/>
+      <c r="D23" s="32" t="n"/>
+      <c r="E23" s="32" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="147" t="inlineStr">
@@ -2870,27 +2558,10 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B24" s="148" t="inlineStr">
-        <is>
-          <t>Acción “Crear incidencia”</t>
-        </is>
-      </c>
-      <c r="C24" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno”, visualizando el Listado de envíos de cualquier tag/estado (excepto incidencias), cuando presione sobre la acción “Crear incidencia”,</t>
-        </is>
-      </c>
-      <c r="D24" s="32" t="inlineStr">
-        <is>
-          <t>Se Activa la HU-011 Crear Incidencia</t>
-        </is>
-      </c>
-      <c r="E24" s="32" t="inlineStr">
-        <is>
-          <t>Acción
-Crear Incidencia</t>
-        </is>
-      </c>
+      <c r="B24" s="148" t="n"/>
+      <c r="C24" s="32" t="n"/>
+      <c r="D24" s="32" t="n"/>
+      <c r="E24" s="32" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="147" t="inlineStr">
@@ -2898,33 +2569,10 @@
           <t>19</t>
         </is>
       </c>
-      <c r="B25" s="148" t="inlineStr">
-        <is>
-          <t>Activar/Desactivar Celdas</t>
-        </is>
-      </c>
-      <c r="C25" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” en cualquiera de los estados y desea visualizar más a detalle los registros de correo interno,</t>
-        </is>
-      </c>
-      <c r="D25" s="32" t="inlineStr">
-        <is>
-          <t>El sistema permitirá al usuario:
-Activar celdas:
-Al activar esta opción  el sistema expandirá la vista de la tabla para mostrar información secundaria de cada registro de correo interno que se está visualizando.
-No se requiere selección de registros específicos, la expansión aplicará a todos los registros visibles en la tabla.
-Desactivar celdas
-Activar la sección "Desactivar Celdas" para regresar a la vista inicial de la tabla. Al presionar sobre esta opción, el sistema ocultará la información secundaria y mostrará nuevamente la vista compacta de la tabla.
-El usuario continuará viendo la misma sección de la tabla que estaba visualizando antes de desactivar la expansión.</t>
-        </is>
-      </c>
-      <c r="E25" s="32" t="inlineStr">
-        <is>
-          <t>Botón:
-Activar Celdas</t>
-        </is>
-      </c>
+      <c r="B25" s="148" t="n"/>
+      <c r="C25" s="32" t="n"/>
+      <c r="D25" s="32" t="n"/>
+      <c r="E25" s="32" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="147" t="inlineStr">
@@ -2932,21 +2580,9 @@
           <t>20</t>
         </is>
       </c>
-      <c r="B26" s="148" t="inlineStr">
-        <is>
-          <t>Ver información secundaria</t>
-        </is>
-      </c>
-      <c r="C26" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y desea visualizar la información secundaria de un envío en específico, al pasar el cursor sobre  dicho envío,</t>
-        </is>
-      </c>
-      <c r="D26" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá expandir la vista del registro y automáticamente mostrar la información secundaria del envío.</t>
-        </is>
-      </c>
+      <c r="B26" s="148" t="n"/>
+      <c r="C26" s="32" t="n"/>
+      <c r="D26" s="32" t="n"/>
       <c r="E26" s="32" t="n"/>
     </row>
     <row r="27">
@@ -2955,42 +2591,10 @@
           <t>21</t>
         </is>
       </c>
-      <c r="B27" s="148" t="inlineStr">
-        <is>
-          <t>Filtros tabla</t>
-        </is>
-      </c>
-      <c r="C27" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” en cualquiera de los estados y presiona sobre Icono filtro (),</t>
-        </is>
-      </c>
-      <c r="D27" s="32" t="inlineStr">
-        <is>
-          <t>Si la sección filtrado está deshabilitada el sistema debe habilitar la sección de filtrado en la tabla. 
-Si la sección filtrado está habilitada el sistema debe deshabilitar la sección de filtrado en la tabla.</t>
-        </is>
-      </c>
-      <c r="E27" s="32" t="inlineStr">
-        <is>
-          <t>Botón
-Filtro
-Tener en cuenta que esto solo será visible cuando la sección de filtrado esté habilitada.
-Filtros:
-ID GIO
-Tipo de envío
-Remitente
-Formato de recogida
-Ubicación recogida
-Destinatario
-Formato de Entrega
-Ubicación Entrega
-Estado
-Botones:
-Borrar
-Aplicar</t>
-        </is>
-      </c>
+      <c r="B27" s="148" t="n"/>
+      <c r="C27" s="32" t="n"/>
+      <c r="D27" s="32" t="n"/>
+      <c r="E27" s="32" t="n"/>
     </row>
     <row r="28" ht="16.2" customHeight="1" s="212">
       <c r="A28" s="147" t="inlineStr">
@@ -2998,24 +2602,9 @@
           <t>22</t>
         </is>
       </c>
-      <c r="B28" s="126" t="inlineStr">
-        <is>
-          <t>Filtros</t>
-        </is>
-      </c>
-      <c r="C28" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y diligencie alguno de los filtros del panel de filtrado,</t>
-        </is>
-      </c>
-      <c r="D28" s="32" t="inlineStr">
-        <is>
-          <t>Estos deben ser un campo de entrada de texto.
-El sistema solo debe permitir escribir caracteres alfanuméricos.
-Por defecto los campos deben estar vacíos.
-Los filtros de texto por defecto deben ser del tipo "Contains" y ser indistintas las mayúsculas y las minúsculas (Case Insensitive) y a los "acentos"  (a=á=ä=à=â) (Accent Insensitive).</t>
-        </is>
-      </c>
+      <c r="B28" s="126" t="n"/>
+      <c r="C28" s="32" t="n"/>
+      <c r="D28" s="32" t="n"/>
       <c r="E28" s="32" t="n"/>
     </row>
     <row r="29" ht="16.2" customHeight="1" s="212">
@@ -3024,21 +2613,9 @@
           <t>23</t>
         </is>
       </c>
-      <c r="B29" s="148" t="inlineStr">
-        <is>
-          <t>Filtro en campo “Estado”</t>
-        </is>
-      </c>
-      <c r="C29" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y ha habilitado el panel de filtrar,  y desee ver los registros por estado,</t>
-        </is>
-      </c>
-      <c r="D29" s="32" t="inlineStr">
-        <is>
-          <t>Por defecto el filtro estará establecido de acuerdo al estado que el usuario ha seleccionado para la visualización del listado y el usuario NO podrá seleccionar ningún otro estado para filtrar.</t>
-        </is>
-      </c>
+      <c r="B29" s="148" t="n"/>
+      <c r="C29" s="32" t="n"/>
+      <c r="D29" s="32" t="n"/>
       <c r="E29" s="32" t="n"/>
     </row>
     <row r="30" ht="16.2" customHeight="1" s="212">
@@ -3047,28 +2624,10 @@
           <t>24</t>
         </is>
       </c>
-      <c r="B30" s="148" t="inlineStr">
-        <is>
-          <t>Aplicar filtros</t>
-        </is>
-      </c>
-      <c r="C30" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno”  y ha habilitado el panel de filtrar, al  dar clic en el botón “Aplicar”,</t>
-        </is>
-      </c>
-      <c r="D30" s="32" t="inlineStr">
-        <is>
-          <t>El sistema debe mostrar en la tabla los registros.
-Al no encontrar registros debe aparecer el mensaje “No existen registros” en la tabla.</t>
-        </is>
-      </c>
-      <c r="E30" s="32" t="inlineStr">
-        <is>
-          <t>Botón:
-Aplicar</t>
-        </is>
-      </c>
+      <c r="B30" s="148" t="n"/>
+      <c r="C30" s="32" t="n"/>
+      <c r="D30" s="32" t="n"/>
+      <c r="E30" s="32" t="n"/>
     </row>
     <row r="31" ht="16.2" customHeight="1" s="212">
       <c r="A31" s="147" t="inlineStr">
@@ -3076,28 +2635,10 @@
           <t>25</t>
         </is>
       </c>
-      <c r="B31" s="148" t="inlineStr">
-        <is>
-          <t>Limpiar filtros</t>
-        </is>
-      </c>
-      <c r="C31" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y ha habilitado el panel de filtrar, al  dar clic en el botón “Borrar” o deshabilita la sección de filtrado,</t>
-        </is>
-      </c>
-      <c r="D31" s="32" t="inlineStr">
-        <is>
-          <t>El sistema debe regresar todos los filtros a su estado por defecto.
-En la tabla deben aparecer todos los registros.</t>
-        </is>
-      </c>
-      <c r="E31" s="32" t="inlineStr">
-        <is>
-          <t>Botón:
-Borrar</t>
-        </is>
-      </c>
+      <c r="B31" s="148" t="n"/>
+      <c r="C31" s="32" t="n"/>
+      <c r="D31" s="32" t="n"/>
+      <c r="E31" s="32" t="n"/>
     </row>
     <row r="32" ht="16.2" customHeight="1" s="212">
       <c r="A32" s="147" t="inlineStr">
@@ -3105,31 +2646,10 @@
           <t>26</t>
         </is>
       </c>
-      <c r="B32" s="148" t="inlineStr">
-        <is>
-          <t>Nuevo envío</t>
-        </is>
-      </c>
-      <c r="C32" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y desea registrar un nuevo envío, al presionar sobre el botón “Nuevo envío”,</t>
-        </is>
-      </c>
-      <c r="D32" s="32" t="inlineStr">
-        <is>
-          <t>El sistema deberá mostrar un menú desplegable con las siguientes opciones:
-Nueva Salida
-Se activa HU-015	Registrar salida
-Nuevo correo interno
-Se Activa HU-020 Registrar Correo Interno</t>
-        </is>
-      </c>
-      <c r="E32" s="32" t="inlineStr">
-        <is>
-          <t>Botón:
-Nuevo envío</t>
-        </is>
-      </c>
+      <c r="B32" s="148" t="n"/>
+      <c r="C32" s="32" t="n"/>
+      <c r="D32" s="32" t="n"/>
+      <c r="E32" s="32" t="n"/>
     </row>
     <row r="33" ht="16.2" customHeight="1" s="212">
       <c r="A33" s="147" t="inlineStr">
@@ -3137,27 +2657,10 @@
           <t>27</t>
         </is>
       </c>
-      <c r="B33" s="148" t="inlineStr">
-        <is>
-          <t>Exportar información</t>
-        </is>
-      </c>
-      <c r="C33" s="148" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno” y desea exportar la información visualizada, cuando hace clic en la opción “Acciones de datos” &gt; “Exportar”</t>
-        </is>
-      </c>
-      <c r="D33" s="148" t="inlineStr">
-        <is>
-          <t>El sistema permitirá exportar la información del listado teniendo en cuenta los filtros que se hayan aplicado. Se activa HU-056 Exportación de datos</t>
-        </is>
-      </c>
-      <c r="E33" s="32" t="inlineStr">
-        <is>
-          <t>Botón:
-Exportar</t>
-        </is>
-      </c>
+      <c r="B33" s="148" t="n"/>
+      <c r="C33" s="148" t="n"/>
+      <c r="D33" s="148" t="n"/>
+      <c r="E33" s="32" t="n"/>
     </row>
     <row r="34" ht="16.2" customHeight="1" s="212">
       <c r="A34" s="147" t="inlineStr">
@@ -3165,22 +2668,9 @@
           <t>28</t>
         </is>
       </c>
-      <c r="B34" s="148" t="inlineStr">
-        <is>
-          <t>Paginado y Desplazamiento en Listados</t>
-        </is>
-      </c>
-      <c r="C34" s="32" t="inlineStr">
-        <is>
-          <t>Dado que el usuario se encuentra en la Pantalla “Envíos Físicos &gt; Correo Interno”  se busca mejorar la visualización de listados en cada estado, cuando el usuario acceda a cualquier lista de estados,</t>
-        </is>
-      </c>
-      <c r="D34" s="32" t="inlineStr">
-        <is>
-          <t>Si la totalidad de los registros no alcanzan a mostrarse en pantalla, la información se mostrará paginada y con barras de desplazamiento. 
-Se activa HU-098  (Paginado de tablas).</t>
-        </is>
-      </c>
+      <c r="B34" s="148" t="n"/>
+      <c r="C34" s="32" t="n"/>
+      <c r="D34" s="32" t="n"/>
       <c r="E34" s="150" t="n"/>
     </row>
     <row r="35" ht="16.2" customHeight="1" s="212">
@@ -16740,7 +16230,7 @@
       <c r="CV127" s="122" t="n"/>
       <c r="CW127" s="122" t="n"/>
     </row>
-    <row r="128">
+    <row r="128" ht="57.6" customHeight="1" s="212">
       <c r="A128" s="99" t="inlineStr">
         <is>
           <t>TITULOS DE LOS PASOS</t>
@@ -17770,8 +17260,8 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="BD11:BD12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="AM11:AM12"/>
-    <mergeCell ref="E11:E12"/>
     <mergeCell ref="BV11:BV12"/>
     <mergeCell ref="BG11:BG12"/>
     <mergeCell ref="BE11:BE12"/>
@@ -17799,7 +17289,7 @@
   </sheetPr>
   <dimension ref="A1:AT731"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -17838,8 +17328,8 @@
     <col width="24.33203125" customWidth="1" style="224" min="40" max="40"/>
     <col width="11.44140625" customWidth="1" style="5" min="41" max="41"/>
     <col width="19.21875" customWidth="1" style="5" min="42" max="42"/>
-    <col width="11.44140625" customWidth="1" style="5" min="43" max="46"/>
-    <col width="11.44140625" customWidth="1" style="5" min="47" max="16384"/>
+    <col width="11.44140625" customWidth="1" style="5" min="43" max="49"/>
+    <col width="11.44140625" customWidth="1" style="5" min="50" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="212">
@@ -26656,8 +26146,8 @@
     <col width="106.21875" customWidth="1" style="50" min="10" max="10"/>
     <col width="6.21875" bestFit="1" customWidth="1" style="50" min="11" max="11"/>
     <col width="17.5546875" customWidth="1" style="50" min="12" max="12"/>
-    <col width="11.44140625" customWidth="1" style="50" min="13" max="16"/>
-    <col width="11.44140625" customWidth="1" style="50" min="17" max="16384"/>
+    <col width="11.44140625" customWidth="1" style="50" min="13" max="19"/>
+    <col width="11.44140625" customWidth="1" style="50" min="20" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customFormat="1" customHeight="1" s="44">
@@ -31111,8 +30601,8 @@
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C7:G7"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C7:G7"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="E3:F3"/>
@@ -31139,8 +30629,8 @@
     <col width="43.33203125" customWidth="1" style="269" min="2" max="2"/>
     <col width="98.33203125" customWidth="1" style="269" min="3" max="3"/>
     <col width="27" customWidth="1" style="269" min="4" max="4"/>
-    <col width="11.44140625" customWidth="1" style="269" min="5" max="8"/>
-    <col width="11.44140625" customWidth="1" style="269" min="9" max="16384"/>
+    <col width="11.44140625" customWidth="1" style="269" min="5" max="11"/>
+    <col width="11.44140625" customWidth="1" style="269" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -31162,7 +30652,7 @@
       <c r="D3" s="208" t="n"/>
     </row>
     <row r="4" ht="14.4" customHeight="1" s="212">
-      <c r="B4" s="273" t="inlineStr">
+      <c r="B4" s="272" t="inlineStr">
         <is>
           <t>INSTRUCCIONES DE DILIGENCIAMIENTO DE LOS CASOS DE PRUEBA</t>
         </is>
@@ -31457,7 +30947,7 @@
       </c>
     </row>
     <row r="24" ht="15" customHeight="1" s="212">
-      <c r="A24" s="272" t="inlineStr">
+      <c r="A24" s="274" t="inlineStr">
         <is>
           <t>Notas Importantes:</t>
         </is>
@@ -31482,7 +30972,7 @@
     </row>
     <row r="26" ht="13.5" customHeight="1" s="212">
       <c r="A26" s="204" t="n"/>
-      <c r="B26" s="274" t="inlineStr">
+      <c r="B26" s="273" t="inlineStr">
         <is>
           <t>Es importante que por cada modificación del documento entre los diferentes actores se cree una nueva versión del documento y diligenciar la hoja de CONTROL DE VERSIONES</t>
         </is>
@@ -31492,7 +30982,7 @@
     </row>
     <row r="27" ht="13.5" customHeight="1" s="212">
       <c r="A27" s="204" t="n"/>
-      <c r="B27" s="274" t="inlineStr">
+      <c r="B27" s="273" t="inlineStr">
         <is>
           <t xml:space="preserve">Los datos que deben ser diligenciados en la pestaña 'DICCIONARIO', deben corresponder al código fuente del software que se va a testear. </t>
         </is>
@@ -31542,11 +31032,11 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A24:A28"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A24:A28"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A8:A13"/>
@@ -31578,8 +31068,8 @@
     <col width="15.5546875" customWidth="1" style="269" min="4" max="4"/>
     <col width="24.5546875" bestFit="1" customWidth="1" style="269" min="5" max="5"/>
     <col width="8.6640625" customWidth="1" style="269" min="6" max="6"/>
-    <col width="11.44140625" customWidth="1" style="269" min="7" max="10"/>
-    <col width="11.44140625" customWidth="1" style="269" min="11" max="16384"/>
+    <col width="11.44140625" customWidth="1" style="269" min="7" max="13"/>
+    <col width="11.44140625" customWidth="1" style="269" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>